<commit_message>
added unit tests for the parser
</commit_message>
<xml_diff>
--- a/doc/routing.xlsx
+++ b/doc/routing.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects.pet\ConsoleTools.Commando\repo\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73A2B05-FBF9-4421-99C1-E37A2DAEC312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA611148-0F1C-439B-99C6-92DCE6355DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{69909FE3-4B00-40CE-B870-8E5B08BB4665}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{69909FE3-4B00-40CE-B870-8E5B08BB4665}"/>
   </bookViews>
   <sheets>
-    <sheet name="routing result" sheetId="1" r:id="rId1"/>
-    <sheet name="command state" sheetId="2" r:id="rId2"/>
+    <sheet name="command match" sheetId="2" r:id="rId1"/>
+    <sheet name="routing result" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>any (0,1,many)</t>
   </si>
@@ -45,85 +45,100 @@
     <t>ok -&gt; execute the named command.</t>
   </si>
   <si>
+    <t>many</t>
+  </si>
+  <si>
+    <t>none -&gt; display the general help</t>
+  </si>
+  <si>
+    <t>ok -&gt; execute the anonymous command.</t>
+  </si>
+  <si>
+    <t>inconclusive -&gt; display info about the multiple anonymous commands (possible argument combinations)</t>
+  </si>
+  <si>
+    <t>inconclusive -&gt; display info about the multiple commands with same name</t>
+  </si>
+  <si>
+    <t>no-match</t>
+  </si>
+  <si>
+    <t>match</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>partial</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>resulted command state</t>
+  </si>
+  <si>
+    <t>routing result</t>
+  </si>
+  <si>
+    <t>any</t>
+  </si>
+  <si>
+    <t>anonymous
+commands matched</t>
+  </si>
+  <si>
     <t>named
-command</t>
-  </si>
-  <si>
-    <t>anonymous
-command</t>
-  </si>
-  <si>
-    <t>many</t>
-  </si>
-  <si>
-    <t>none -&gt; display the general help</t>
-  </si>
-  <si>
-    <t>ok -&gt; execute the anonymous command.</t>
-  </si>
-  <si>
-    <t>inconclusive -&gt; display info about the multiple anonymous commands (possible argument combinations)</t>
-  </si>
-  <si>
-    <t>inconclusive -&gt; display info about the multiple commands with same name</t>
-  </si>
-  <si>
-    <t>parameters
-match</t>
-  </si>
-  <si>
-    <t>unused
-parameters</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>no-match</t>
-  </si>
-  <si>
-    <t>match</t>
-  </si>
-  <si>
-    <t>all</t>
-  </si>
-  <si>
-    <t>partial</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>resulted command state</t>
-  </si>
-  <si>
-    <t>routing result</t>
-  </si>
-  <si>
-    <t>partial-match</t>
-  </si>
-  <si>
-    <t>full-match</t>
-  </si>
-  <si>
-    <t>any</t>
+commands matched</t>
   </si>
   <si>
     <t>command
-name</t>
+name matched</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>used
+arguments</t>
+  </si>
+  <si>
+    <t>impossible</t>
+  </si>
+  <si>
+    <t>command has parameters</t>
+  </si>
+  <si>
+    <t>arguments are provided</t>
+  </si>
+  <si>
+    <t>parameters are
+populated</t>
+  </si>
+  <si>
+    <t>full-match (weak)</t>
+  </si>
+  <si>
+    <t>full-match (strong)</t>
+  </si>
+  <si>
+    <t>partial-match (strong)</t>
+  </si>
+  <si>
+    <t>partial-match (weak)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,13 +156,57 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -168,13 +227,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -188,14 +253,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="5" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="7" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="4" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="6" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="8">
+    <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="3" builtinId="39"/>
+    <cellStyle name="40% - Accent4" xfId="4" builtinId="43"/>
+    <cellStyle name="40% - Accent6" xfId="6" builtinId="51"/>
+    <cellStyle name="60% - Accent4" xfId="5" builtinId="44"/>
+    <cellStyle name="60% - Accent6" xfId="7" builtinId="52"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
@@ -508,28 +601,242 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9AE9199-0C98-477A-8BA0-6E848EDEA6D2}">
+  <dimension ref="B2:G13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="6" width="21.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="71.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" s="2" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="D3:D9"/>
+    <mergeCell ref="B3:B12"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="C3:C10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6827584B-C955-473B-A95A-99B889C06C3F}">
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="21.85546875" style="1" customWidth="1"/>
+    <col min="2" max="3" width="27.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="71.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" s="2" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -548,10 +855,10 @@
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -562,7 +869,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -573,170 +880,21 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9AE9199-0C98-477A-8BA0-6E848EDEA6D2}">
-  <dimension ref="B2:E12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="4" width="21.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="71.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:5" s="2" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
-      <c r="C7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B3:B8"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>